<commit_message>
adding the products tiles in live plants page
</commit_message>
<xml_diff>
--- a/data/master_item_list.xlsx
+++ b/data/master_item_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankush\Desktop\bhumij_work\website_flask\bhumij_flask_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA6F341-29A7-4EBD-A67B-87EB2C33E5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18B3E3C-BF82-43DA-856A-793F740E90C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
-    <t>Item Name</t>
-  </si>
-  <si>
-    <t>Main Category</t>
-  </si>
-  <si>
     <t>Aglaonema Snow White</t>
   </si>
   <si>
@@ -81,7 +75,13 @@
     <t>s</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>item_name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>main_category</t>
   </si>
 </sst>
 </file>
@@ -145,22 +145,22 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,21 +458,21 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>151</v>
@@ -480,10 +480,10 @@
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>141</v>
@@ -491,24 +491,24 @@
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>81</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <v>71</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>131</v>
@@ -527,10 +527,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
         <v>111</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
         <v>41</v>
@@ -549,10 +549,10 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>71</v>
@@ -560,10 +560,10 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
         <v>99</v>
@@ -571,10 +571,10 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>41</v>
@@ -582,10 +582,10 @@
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>71</v>
@@ -593,10 +593,10 @@
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
         <v>33</v>
@@ -604,10 +604,10 @@
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
         <v>35</v>
@@ -615,10 +615,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
         <v>41</v>

</xml_diff>